<commit_message>
Committing changes in testcases
</commit_message>
<xml_diff>
--- a/com.supermarket/src/main/resources/excelFile/TestData.xlsx
+++ b/com.supermarket/src/main/resources/excelFile/TestData.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="12060" windowHeight="2655"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>Username</t>
   </si>
@@ -43,6 +44,15 @@
   </si>
   <si>
     <t>Edited Username</t>
+  </si>
+  <si>
+    <t>Editoffercode</t>
+  </si>
+  <si>
+    <t>EditPercentageValue</t>
+  </si>
+  <si>
+    <t>Edit Percentage</t>
   </si>
 </sst>
 </file>
@@ -86,9 +96,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -390,10 +401,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -444,6 +455,27 @@
       </c>
       <c r="B7" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="2">
+        <v>0.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>